<commit_message>
Analysis with self-ratings in ESS
</commit_message>
<xml_diff>
--- a/data/processed/CHES_2014.vote.keys.combined.xlsx
+++ b/data/processed/CHES_2014.vote.keys.combined.xlsx
@@ -137,15 +137,15 @@
     <t xml:space="preserve">Open VLD</t>
   </si>
   <si>
+    <t xml:space="preserve">PS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PVDA+</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parti Populaire</t>
   </si>
   <si>
-    <t xml:space="preserve">PS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PVDA+</t>
-  </si>
-  <si>
     <t xml:space="preserve">SP.A</t>
   </si>
   <si>
@@ -194,24 +194,24 @@
     <t xml:space="preserve">ANO 2011</t>
   </si>
   <si>
+    <t xml:space="preserve">KDU-ČSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KSČM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ODS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TOP 09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Úsvit přímé demokracie Tomia Okamury</t>
+  </si>
+  <si>
     <t xml:space="preserve">ČSSD</t>
   </si>
   <si>
-    <t xml:space="preserve">KDU-ČSL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KSČM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ODS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOP 09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Úsvit přímé demokracie Tomia Okamury</t>
-  </si>
-  <si>
     <t xml:space="preserve">DE</t>
   </si>
   <si>
@@ -359,13 +359,13 @@
     <t xml:space="preserve">Nouveau Centre</t>
   </si>
   <si>
+    <t xml:space="preserve">PR (Parti Radical Valoisien)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PS (Parti Socialiste)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parti Radical de Gauche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR (Parti Radical Valoisien)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PS (Parti Socialiste)</t>
   </si>
   <si>
     <t xml:space="preserve">UMP (Union pour un Mouvement Populaire)</t>
@@ -2103,73 +2103,73 @@
         <v>41</v>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D16" t="n">
-        <v>7.75</v>
+        <v>2.5999999</v>
       </c>
       <c r="E16" t="n">
-        <v>8.5</v>
+        <v>2.4000001</v>
       </c>
       <c r="F16" t="n">
-        <v>7.5</v>
+        <v>3.4000001</v>
       </c>
       <c r="G16" t="n">
-        <v>7</v>
+        <v>2.4000001</v>
       </c>
       <c r="H16" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="I16" t="n">
-        <v>6.5</v>
+        <v>1.8</v>
       </c>
       <c r="J16" t="n">
-        <v>7</v>
+        <v>1.75</v>
       </c>
       <c r="K16" t="n">
-        <v>8.5</v>
+        <v>2.2</v>
       </c>
       <c r="L16" t="n">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="M16" t="n">
+        <v>1</v>
+      </c>
+      <c r="N16" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="O16" t="n">
         <v>2</v>
       </c>
-      <c r="N16" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="O16" t="n">
-        <v>9</v>
-      </c>
       <c r="P16" t="n">
-        <v>6</v>
+        <v>3.3333333</v>
       </c>
       <c r="Q16" t="n">
-        <v>7.5</v>
+        <v>3.8</v>
       </c>
       <c r="R16" t="n">
-        <v>8.5</v>
+        <v>6.5999999</v>
       </c>
       <c r="S16" t="n">
-        <v>6</v>
+        <v>5.8000002</v>
       </c>
       <c r="T16" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="U16" t="n">
-        <v>10</v>
+        <v>2.25</v>
       </c>
       <c r="V16" t="n">
-        <v>8.8000002</v>
+        <v>8.3999996</v>
       </c>
       <c r="W16" t="n">
-        <v>6.1999998</v>
+        <v>3.2</v>
       </c>
       <c r="X16" t="n">
-        <v>6.5</v>
+        <v>2.5999999</v>
       </c>
       <c r="Y16" t="n">
-        <v>5.3333335</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="17">
@@ -2180,73 +2180,73 @@
         <v>42</v>
       </c>
       <c r="C17" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>2.5999999</v>
+        <v>0.40000001</v>
       </c>
       <c r="E17" t="n">
-        <v>2.4000001</v>
+        <v>0.2</v>
       </c>
       <c r="F17" t="n">
-        <v>3.4000001</v>
+        <v>2.8</v>
       </c>
       <c r="G17" t="n">
-        <v>2.4000001</v>
+        <v>0.2</v>
       </c>
       <c r="H17" t="n">
+        <v>0.40000001</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K17" t="n">
         <v>2</v>
       </c>
-      <c r="I17" t="n">
+      <c r="L17" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.80000001</v>
+      </c>
+      <c r="N17" t="n">
         <v>1.8</v>
       </c>
-      <c r="J17" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="K17" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="L17" t="n">
+      <c r="O17" t="n">
         <v>1.6</v>
       </c>
-      <c r="M17" t="n">
+      <c r="P17" t="n">
+        <v>2.6666667</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>4.5999999</v>
+      </c>
+      <c r="R17" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="S17" t="n">
+        <v>7.8000002</v>
+      </c>
+      <c r="T17" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="U17" t="n">
         <v>1</v>
       </c>
-      <c r="N17" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="O17" t="n">
-        <v>2</v>
-      </c>
-      <c r="P17" t="n">
-        <v>3.3333333</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="R17" t="n">
-        <v>6.5999999</v>
-      </c>
-      <c r="S17" t="n">
-        <v>5.8000002</v>
-      </c>
-      <c r="T17" t="n">
-        <v>2</v>
-      </c>
-      <c r="U17" t="n">
-        <v>2.25</v>
-      </c>
       <c r="V17" t="n">
+        <v>8.6000004</v>
+      </c>
+      <c r="W17" t="n">
+        <v>4.4000001</v>
+      </c>
+      <c r="X17" t="n">
         <v>8.3999996</v>
       </c>
-      <c r="W17" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="X17" t="n">
-        <v>2.5999999</v>
-      </c>
       <c r="Y17" t="n">
-        <v>2.25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18">
@@ -2257,73 +2257,73 @@
         <v>43</v>
       </c>
       <c r="C18" t="n">
+        <v>15</v>
+      </c>
+      <c r="D18" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="E18" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="F18" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7</v>
+      </c>
+      <c r="H18" t="n">
+        <v>7</v>
+      </c>
+      <c r="I18" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="J18" t="n">
+        <v>7</v>
+      </c>
+      <c r="K18" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="L18" t="n">
+        <v>7</v>
+      </c>
+      <c r="M18" t="n">
+        <v>2</v>
+      </c>
+      <c r="N18" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="O18" t="n">
+        <v>9</v>
+      </c>
+      <c r="P18" t="n">
         <v>6</v>
       </c>
-      <c r="D18" t="n">
-        <v>0.40000001</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F18" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="G18" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.40000001</v>
-      </c>
-      <c r="I18" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="K18" t="n">
-        <v>2</v>
-      </c>
-      <c r="L18" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="M18" t="n">
-        <v>0.80000001</v>
-      </c>
-      <c r="N18" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="O18" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="P18" t="n">
-        <v>2.6666667</v>
-      </c>
       <c r="Q18" t="n">
-        <v>4.5999999</v>
+        <v>7.5</v>
       </c>
       <c r="R18" t="n">
-        <v>9.25</v>
+        <v>8.5</v>
       </c>
       <c r="S18" t="n">
-        <v>7.8000002</v>
+        <v>6</v>
       </c>
       <c r="T18" t="n">
-        <v>1.6</v>
+        <v>9</v>
       </c>
       <c r="U18" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="V18" t="n">
-        <v>8.6000004</v>
+        <v>8.8000002</v>
       </c>
       <c r="W18" t="n">
-        <v>4.4000001</v>
+        <v>6.1999998</v>
       </c>
       <c r="X18" t="n">
-        <v>8.3999996</v>
+        <v>6.5</v>
       </c>
       <c r="Y18" t="n">
-        <v>6</v>
+        <v>5.3333335</v>
       </c>
     </row>
     <row r="19">
@@ -3412,73 +3412,73 @@
         <v>60</v>
       </c>
       <c r="C33" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>3.1428571</v>
+        <v>5.9285712</v>
       </c>
       <c r="E33" t="n">
-        <v>2.7142856</v>
+        <v>5.5714288</v>
       </c>
       <c r="F33" t="n">
-        <v>4.4285712</v>
+        <v>7.6428571</v>
       </c>
       <c r="G33" t="n">
-        <v>2.6363637</v>
+        <v>4.9000001</v>
       </c>
       <c r="H33" t="n">
-        <v>3.8333333</v>
+        <v>4.8333335</v>
       </c>
       <c r="I33" t="n">
-        <v>2.8461537</v>
+        <v>4.9166665</v>
       </c>
       <c r="J33" t="n">
-        <v>2.8461537</v>
+        <v>4.7692308</v>
       </c>
       <c r="K33" t="n">
-        <v>4.8333335</v>
+        <v>7.3333335</v>
       </c>
       <c r="L33" t="n">
-        <v>3.3076923</v>
+        <v>8.1538458</v>
       </c>
       <c r="M33" t="n">
-        <v>2.7692308</v>
+        <v>9.1538458</v>
       </c>
       <c r="N33" t="n">
-        <v>4.3333335</v>
+        <v>7</v>
       </c>
       <c r="O33" t="n">
-        <v>4.25</v>
+        <v>7.7272725</v>
       </c>
       <c r="P33" t="n">
-        <v>4.9166665</v>
+        <v>8</v>
       </c>
       <c r="Q33" t="n">
-        <v>5.6923075</v>
+        <v>4.5833335</v>
       </c>
       <c r="R33" t="n">
-        <v>4.5</v>
+        <v>3.8181818</v>
       </c>
       <c r="S33" t="n">
-        <v>4.5833335</v>
+        <v>3</v>
       </c>
       <c r="T33" t="n">
-        <v>4.6923075</v>
+        <v>5.75</v>
       </c>
       <c r="U33" t="n">
         <v>5.0769229</v>
       </c>
       <c r="V33" t="n">
-        <v>7.8571429</v>
+        <v>6.2142859</v>
       </c>
       <c r="W33" t="n">
-        <v>3.1428571</v>
+        <v>7.2142859</v>
       </c>
       <c r="X33" t="n">
-        <v>1.5</v>
+        <v>2.4615386</v>
       </c>
       <c r="Y33" t="n">
-        <v>5.2307692</v>
+        <v>5.5384617</v>
       </c>
     </row>
     <row r="34">
@@ -3489,73 +3489,73 @@
         <v>61</v>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D34" t="n">
-        <v>5.9285712</v>
+        <v>1.0714285</v>
       </c>
       <c r="E34" t="n">
-        <v>5.5714288</v>
+        <v>1</v>
       </c>
       <c r="F34" t="n">
-        <v>7.6428571</v>
+        <v>6.5714288</v>
       </c>
       <c r="G34" t="n">
-        <v>4.9000001</v>
+        <v>1.0909091</v>
       </c>
       <c r="H34" t="n">
-        <v>4.8333335</v>
+        <v>2.0833333</v>
       </c>
       <c r="I34" t="n">
-        <v>4.9166665</v>
+        <v>0.84615386</v>
       </c>
       <c r="J34" t="n">
-        <v>4.7692308</v>
+        <v>0.61538464</v>
       </c>
       <c r="K34" t="n">
-        <v>7.3333335</v>
+        <v>7</v>
       </c>
       <c r="L34" t="n">
-        <v>8.1538458</v>
+        <v>5.6923075</v>
       </c>
       <c r="M34" t="n">
-        <v>9.1538458</v>
+        <v>0.46153846</v>
       </c>
       <c r="N34" t="n">
-        <v>7</v>
+        <v>6.6666665</v>
       </c>
       <c r="O34" t="n">
-        <v>7.7272725</v>
+        <v>6.8000002</v>
       </c>
       <c r="P34" t="n">
-        <v>8</v>
+        <v>6.0833335</v>
       </c>
       <c r="Q34" t="n">
-        <v>4.5833335</v>
+        <v>6.9166665</v>
       </c>
       <c r="R34" t="n">
-        <v>3.8181818</v>
+        <v>6.3000002</v>
       </c>
       <c r="S34" t="n">
-        <v>3</v>
+        <v>8.416667</v>
       </c>
       <c r="T34" t="n">
-        <v>5.75</v>
+        <v>6.181818</v>
       </c>
       <c r="U34" t="n">
-        <v>5.0769229</v>
+        <v>7.6153846</v>
       </c>
       <c r="V34" t="n">
-        <v>6.2142859</v>
+        <v>7.2857141</v>
       </c>
       <c r="W34" t="n">
-        <v>7.2142859</v>
+        <v>3.6153846</v>
       </c>
       <c r="X34" t="n">
-        <v>2.4615386</v>
+        <v>5.6923075</v>
       </c>
       <c r="Y34" t="n">
-        <v>5.5384617</v>
+        <v>5.4615383</v>
       </c>
     </row>
     <row r="35">
@@ -3566,73 +3566,73 @@
         <v>62</v>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D35" t="n">
-        <v>1.0714285</v>
+        <v>8</v>
       </c>
       <c r="E35" t="n">
-        <v>1</v>
+        <v>8.1428576</v>
       </c>
       <c r="F35" t="n">
-        <v>6.5714288</v>
+        <v>6</v>
       </c>
       <c r="G35" t="n">
-        <v>1.0909091</v>
+        <v>8.181818</v>
       </c>
       <c r="H35" t="n">
-        <v>2.0833333</v>
+        <v>7.5</v>
       </c>
       <c r="I35" t="n">
-        <v>0.84615386</v>
+        <v>7.9166665</v>
       </c>
       <c r="J35" t="n">
-        <v>0.61538464</v>
+        <v>7.9166665</v>
       </c>
       <c r="K35" t="n">
-        <v>7</v>
+        <v>5.0833335</v>
       </c>
       <c r="L35" t="n">
-        <v>5.6923075</v>
+        <v>5.5</v>
       </c>
       <c r="M35" t="n">
-        <v>0.46153846</v>
+        <v>5.2307692</v>
       </c>
       <c r="N35" t="n">
+        <v>7.875</v>
+      </c>
+      <c r="O35" t="n">
+        <v>7.4166665</v>
+      </c>
+      <c r="P35" t="n">
+        <v>3.4166667</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>7.5384617</v>
+      </c>
+      <c r="R35" t="n">
+        <v>6.3636365</v>
+      </c>
+      <c r="S35" t="n">
+        <v>2.4166667</v>
+      </c>
+      <c r="T35" t="n">
         <v>6.6666665</v>
       </c>
-      <c r="O35" t="n">
-        <v>6.8000002</v>
-      </c>
-      <c r="P35" t="n">
-        <v>6.0833335</v>
-      </c>
-      <c r="Q35" t="n">
-        <v>6.9166665</v>
-      </c>
-      <c r="R35" t="n">
-        <v>6.3000002</v>
-      </c>
-      <c r="S35" t="n">
-        <v>8.416667</v>
-      </c>
-      <c r="T35" t="n">
-        <v>6.181818</v>
-      </c>
       <c r="U35" t="n">
-        <v>7.6153846</v>
+        <v>7.4615383</v>
       </c>
       <c r="V35" t="n">
-        <v>7.2857141</v>
+        <v>7.8571429</v>
       </c>
       <c r="W35" t="n">
-        <v>3.6153846</v>
+        <v>5.2142859</v>
       </c>
       <c r="X35" t="n">
-        <v>5.6923075</v>
+        <v>2.1538463</v>
       </c>
       <c r="Y35" t="n">
-        <v>5.4615383</v>
+        <v>3.1538463</v>
       </c>
     </row>
     <row r="36">
@@ -3643,73 +3643,73 @@
         <v>63</v>
       </c>
       <c r="C36" t="n">
+        <v>3</v>
+      </c>
+      <c r="D36" t="n">
+        <v>7.2142859</v>
+      </c>
+      <c r="E36" t="n">
+        <v>7.8571429</v>
+      </c>
+      <c r="F36" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="G36" t="n">
+        <v>7.909091</v>
+      </c>
+      <c r="H36" t="n">
+        <v>7.25</v>
+      </c>
+      <c r="I36" t="n">
+        <v>7.6153846</v>
+      </c>
+      <c r="J36" t="n">
+        <v>7.6923075</v>
+      </c>
+      <c r="K36" t="n">
+        <v>4.0833335</v>
+      </c>
+      <c r="L36" t="n">
+        <v>4.3846154</v>
+      </c>
+      <c r="M36" t="n">
+        <v>6.7692308</v>
+      </c>
+      <c r="N36" t="n">
         <v>5</v>
       </c>
-      <c r="D36" t="n">
-        <v>8</v>
-      </c>
-      <c r="E36" t="n">
-        <v>8.1428576</v>
-      </c>
-      <c r="F36" t="n">
+      <c r="O36" t="n">
         <v>6</v>
       </c>
-      <c r="G36" t="n">
-        <v>8.181818</v>
-      </c>
-      <c r="H36" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="I36" t="n">
-        <v>7.9166665</v>
-      </c>
-      <c r="J36" t="n">
-        <v>7.9166665</v>
-      </c>
-      <c r="K36" t="n">
-        <v>5.0833335</v>
-      </c>
-      <c r="L36" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="M36" t="n">
-        <v>5.2307692</v>
-      </c>
-      <c r="N36" t="n">
-        <v>7.875</v>
-      </c>
-      <c r="O36" t="n">
-        <v>7.4166665</v>
-      </c>
       <c r="P36" t="n">
-        <v>3.4166667</v>
+        <v>3.3333333</v>
       </c>
       <c r="Q36" t="n">
-        <v>7.5384617</v>
+        <v>6.25</v>
       </c>
       <c r="R36" t="n">
-        <v>6.3636365</v>
+        <v>4</v>
       </c>
       <c r="S36" t="n">
-        <v>2.4166667</v>
+        <v>2.25</v>
       </c>
       <c r="T36" t="n">
-        <v>6.6666665</v>
+        <v>4.75</v>
       </c>
       <c r="U36" t="n">
-        <v>7.4615383</v>
+        <v>3.7692308</v>
       </c>
       <c r="V36" t="n">
-        <v>7.8571429</v>
+        <v>7.7142859</v>
       </c>
       <c r="W36" t="n">
-        <v>5.2142859</v>
+        <v>4.5714288</v>
       </c>
       <c r="X36" t="n">
-        <v>2.1538463</v>
+        <v>1.9230769</v>
       </c>
       <c r="Y36" t="n">
-        <v>3.1538463</v>
+        <v>5.0769229</v>
       </c>
     </row>
     <row r="37">
@@ -3720,73 +3720,73 @@
         <v>64</v>
       </c>
       <c r="C37" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D37" t="n">
-        <v>7.2142859</v>
+        <v>7.6923075</v>
       </c>
       <c r="E37" t="n">
-        <v>7.8571429</v>
+        <v>5.3333335</v>
       </c>
       <c r="F37" t="n">
+        <v>7.7142859</v>
+      </c>
+      <c r="G37" t="n">
+        <v>4</v>
+      </c>
+      <c r="H37" t="n">
+        <v>4.4285712</v>
+      </c>
+      <c r="I37" t="n">
+        <v>4</v>
+      </c>
+      <c r="J37" t="n">
         <v>5.5</v>
       </c>
-      <c r="G37" t="n">
-        <v>7.909091</v>
-      </c>
-      <c r="H37" t="n">
-        <v>7.25</v>
-      </c>
-      <c r="I37" t="n">
-        <v>7.6153846</v>
-      </c>
-      <c r="J37" t="n">
-        <v>7.6923075</v>
-      </c>
       <c r="K37" t="n">
-        <v>4.0833335</v>
+        <v>8.583333</v>
       </c>
       <c r="L37" t="n">
-        <v>4.3846154</v>
+        <v>8.181818</v>
       </c>
       <c r="M37" t="n">
-        <v>6.7692308</v>
+        <v>3.1666667</v>
       </c>
       <c r="N37" t="n">
-        <v>5</v>
+        <v>9.3999996</v>
       </c>
       <c r="O37" t="n">
-        <v>6</v>
+        <v>9.666667</v>
       </c>
       <c r="P37" t="n">
-        <v>3.3333333</v>
+        <v>6.4285712</v>
       </c>
       <c r="Q37" t="n">
-        <v>6.25</v>
+        <v>6.5555553</v>
       </c>
       <c r="R37" t="n">
+        <v>4.1666665</v>
+      </c>
+      <c r="S37" t="n">
+        <v>6.6999998</v>
+      </c>
+      <c r="T37" t="n">
+        <v>9.6153851</v>
+      </c>
+      <c r="U37" t="n">
+        <v>9.2307692</v>
+      </c>
+      <c r="V37" t="n">
         <v>4</v>
       </c>
-      <c r="S37" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="T37" t="n">
-        <v>4.75</v>
-      </c>
-      <c r="U37" t="n">
-        <v>3.7692308</v>
-      </c>
-      <c r="V37" t="n">
-        <v>7.7142859</v>
-      </c>
       <c r="W37" t="n">
-        <v>4.5714288</v>
+        <v>6.2307692</v>
       </c>
       <c r="X37" t="n">
-        <v>1.9230769</v>
+        <v>9.4615383</v>
       </c>
       <c r="Y37" t="n">
-        <v>5.0769229</v>
+        <v>8.6153851</v>
       </c>
     </row>
     <row r="38">
@@ -3797,73 +3797,73 @@
         <v>65</v>
       </c>
       <c r="C38" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D38" t="n">
-        <v>7.6923075</v>
+        <v>3.1428571</v>
       </c>
       <c r="E38" t="n">
-        <v>5.3333335</v>
+        <v>2.7142856</v>
       </c>
       <c r="F38" t="n">
-        <v>7.7142859</v>
+        <v>4.4285712</v>
       </c>
       <c r="G38" t="n">
-        <v>4</v>
+        <v>2.6363637</v>
       </c>
       <c r="H38" t="n">
-        <v>4.4285712</v>
+        <v>3.8333333</v>
       </c>
       <c r="I38" t="n">
-        <v>4</v>
+        <v>2.8461537</v>
       </c>
       <c r="J38" t="n">
-        <v>5.5</v>
+        <v>2.8461537</v>
       </c>
       <c r="K38" t="n">
-        <v>8.583333</v>
+        <v>4.8333335</v>
       </c>
       <c r="L38" t="n">
-        <v>8.181818</v>
+        <v>3.3076923</v>
       </c>
       <c r="M38" t="n">
-        <v>3.1666667</v>
+        <v>2.7692308</v>
       </c>
       <c r="N38" t="n">
-        <v>9.3999996</v>
+        <v>4.3333335</v>
       </c>
       <c r="O38" t="n">
-        <v>9.666667</v>
+        <v>4.25</v>
       </c>
       <c r="P38" t="n">
-        <v>6.4285712</v>
+        <v>4.9166665</v>
       </c>
       <c r="Q38" t="n">
-        <v>6.5555553</v>
+        <v>5.6923075</v>
       </c>
       <c r="R38" t="n">
-        <v>4.1666665</v>
+        <v>4.5</v>
       </c>
       <c r="S38" t="n">
-        <v>6.6999998</v>
+        <v>4.5833335</v>
       </c>
       <c r="T38" t="n">
-        <v>9.6153851</v>
+        <v>4.6923075</v>
       </c>
       <c r="U38" t="n">
-        <v>9.2307692</v>
+        <v>5.0769229</v>
       </c>
       <c r="V38" t="n">
-        <v>4</v>
+        <v>7.8571429</v>
       </c>
       <c r="W38" t="n">
-        <v>6.2307692</v>
+        <v>3.1428571</v>
       </c>
       <c r="X38" t="n">
-        <v>9.4615383</v>
+        <v>1.5</v>
       </c>
       <c r="Y38" t="n">
-        <v>8.6153851</v>
+        <v>5.2307692</v>
       </c>
     </row>
     <row r="39">
@@ -7260,73 +7260,73 @@
         <v>115</v>
       </c>
       <c r="C83" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D83" t="n">
-        <v>3.8181818</v>
+        <v>6.1428571</v>
       </c>
       <c r="E83" t="n">
-        <v>3.75</v>
+        <v>6.5</v>
       </c>
       <c r="F83" t="n">
-        <v>3.4166667</v>
+        <v>5.8571429</v>
       </c>
       <c r="G83" t="n">
-        <v>3.4444444</v>
+        <v>6.3333335</v>
       </c>
       <c r="H83" t="n">
-        <v>3.8</v>
+        <v>5.8333335</v>
       </c>
       <c r="I83" t="n">
-        <v>2.7777777</v>
+        <v>6</v>
       </c>
       <c r="J83" t="n">
-        <v>3.5454545</v>
+        <v>5.8333335</v>
       </c>
       <c r="K83" t="n">
-        <v>3.625</v>
+        <v>5.6666665</v>
       </c>
       <c r="L83" t="n">
-        <v>2</v>
+        <v>4.8333335</v>
       </c>
       <c r="M83" t="n">
-        <v>1.7272727</v>
+        <v>3.8333333</v>
       </c>
       <c r="N83" t="n">
+        <v>6.4000001</v>
+      </c>
+      <c r="O83" t="n">
+        <v>6.1666665</v>
+      </c>
+      <c r="P83" t="n">
+        <v>5.4000001</v>
+      </c>
+      <c r="Q83" t="n">
+        <v>6.6666665</v>
+      </c>
+      <c r="R83" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="S83" t="n">
+        <v>4.4000001</v>
+      </c>
+      <c r="T83" t="n">
+        <v>5.8000002</v>
+      </c>
+      <c r="U83" t="n">
+        <v>5.8333335</v>
+      </c>
+      <c r="V83" t="n">
+        <v>7.181818</v>
+      </c>
+      <c r="W83" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="X83" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Y83" t="n">
         <v>4</v>
-      </c>
-      <c r="O83" t="n">
-        <v>5</v>
-      </c>
-      <c r="P83" t="n">
-        <v>5.1666665</v>
-      </c>
-      <c r="Q83" t="n">
-        <v>5.3000002</v>
-      </c>
-      <c r="R83" t="n">
-        <v>3.3333333</v>
-      </c>
-      <c r="S83" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="T83" t="n">
-        <v>4</v>
-      </c>
-      <c r="U83" t="n">
-        <v>4</v>
-      </c>
-      <c r="V83" t="n">
-        <v>6.6363635</v>
-      </c>
-      <c r="W83" t="n">
-        <v>6.4545455</v>
-      </c>
-      <c r="X83" t="n">
-        <v>3.7777777</v>
-      </c>
-      <c r="Y83" t="n">
-        <v>3.5</v>
       </c>
     </row>
     <row r="84">
@@ -7337,73 +7337,73 @@
         <v>116</v>
       </c>
       <c r="C84" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D84" t="n">
-        <v>6.1428571</v>
+        <v>3.8333333</v>
       </c>
       <c r="E84" t="n">
-        <v>6.5</v>
+        <v>3.8333333</v>
       </c>
       <c r="F84" t="n">
-        <v>5.8571429</v>
+        <v>3.3636363</v>
       </c>
       <c r="G84" t="n">
-        <v>6.3333335</v>
+        <v>3.8181818</v>
       </c>
       <c r="H84" t="n">
-        <v>5.8333335</v>
+        <v>4.2727275</v>
       </c>
       <c r="I84" t="n">
-        <v>6</v>
+        <v>3.090909</v>
       </c>
       <c r="J84" t="n">
-        <v>5.8333335</v>
+        <v>3.8181818</v>
       </c>
       <c r="K84" t="n">
-        <v>5.6666665</v>
+        <v>3.909091</v>
       </c>
       <c r="L84" t="n">
-        <v>4.8333335</v>
+        <v>1.9090909</v>
       </c>
       <c r="M84" t="n">
-        <v>3.8333333</v>
+        <v>1.9090909</v>
       </c>
       <c r="N84" t="n">
-        <v>6.4000001</v>
+        <v>4.6999998</v>
       </c>
       <c r="O84" t="n">
-        <v>6.1666665</v>
+        <v>4.7272725</v>
       </c>
       <c r="P84" t="n">
-        <v>5.4000001</v>
+        <v>3.3333333</v>
       </c>
       <c r="Q84" t="n">
-        <v>6.6666665</v>
+        <v>5.3636365</v>
       </c>
       <c r="R84" t="n">
-        <v>4.5</v>
+        <v>3.3</v>
       </c>
       <c r="S84" t="n">
-        <v>4.4000001</v>
+        <v>3.3</v>
       </c>
       <c r="T84" t="n">
-        <v>5.8000002</v>
+        <v>3.7272727</v>
       </c>
       <c r="U84" t="n">
-        <v>5.8333335</v>
+        <v>4.2727275</v>
       </c>
       <c r="V84" t="n">
-        <v>7.181818</v>
+        <v>7.0833335</v>
       </c>
       <c r="W84" t="n">
-        <v>5.5</v>
+        <v>6.5454545</v>
       </c>
       <c r="X84" t="n">
-        <v>3.5</v>
+        <v>3.2</v>
       </c>
       <c r="Y84" t="n">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="85">
@@ -7414,73 +7414,73 @@
         <v>117</v>
       </c>
       <c r="C85" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D85" t="n">
-        <v>3.8333333</v>
+        <v>3.8181818</v>
       </c>
       <c r="E85" t="n">
-        <v>3.8333333</v>
+        <v>3.75</v>
       </c>
       <c r="F85" t="n">
-        <v>3.3636363</v>
+        <v>3.4166667</v>
       </c>
       <c r="G85" t="n">
-        <v>3.8181818</v>
+        <v>3.4444444</v>
       </c>
       <c r="H85" t="n">
-        <v>4.2727275</v>
+        <v>3.8</v>
       </c>
       <c r="I85" t="n">
-        <v>3.090909</v>
+        <v>2.7777777</v>
       </c>
       <c r="J85" t="n">
-        <v>3.8181818</v>
+        <v>3.5454545</v>
       </c>
       <c r="K85" t="n">
-        <v>3.909091</v>
+        <v>3.625</v>
       </c>
       <c r="L85" t="n">
-        <v>1.9090909</v>
+        <v>2</v>
       </c>
       <c r="M85" t="n">
-        <v>1.9090909</v>
+        <v>1.7272727</v>
       </c>
       <c r="N85" t="n">
-        <v>4.6999998</v>
+        <v>4</v>
       </c>
       <c r="O85" t="n">
-        <v>4.7272725</v>
+        <v>5</v>
       </c>
       <c r="P85" t="n">
+        <v>5.1666665</v>
+      </c>
+      <c r="Q85" t="n">
+        <v>5.3000002</v>
+      </c>
+      <c r="R85" t="n">
         <v>3.3333333</v>
       </c>
-      <c r="Q85" t="n">
-        <v>5.3636365</v>
-      </c>
-      <c r="R85" t="n">
-        <v>3.3</v>
-      </c>
       <c r="S85" t="n">
-        <v>3.3</v>
+        <v>4.25</v>
       </c>
       <c r="T85" t="n">
-        <v>3.7272727</v>
+        <v>4</v>
       </c>
       <c r="U85" t="n">
-        <v>4.2727275</v>
+        <v>4</v>
       </c>
       <c r="V85" t="n">
-        <v>7.0833335</v>
+        <v>6.6363635</v>
       </c>
       <c r="W85" t="n">
-        <v>6.5454545</v>
+        <v>6.4545455</v>
       </c>
       <c r="X85" t="n">
-        <v>3.2</v>
+        <v>3.7777777</v>
       </c>
       <c r="Y85" t="n">
-        <v>3.7</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="86">

</xml_diff>